<commit_message>
Groups expenses and split
</commit_message>
<xml_diff>
--- a/DOCS/api_endpoints.xlsx
+++ b/DOCS/api_endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\287928\Desktop\Fianance\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D450FC75-52B0-4AB1-AE2D-BAA985D87E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5CCBF2-2BBA-4A20-89C1-30B2FDCFFBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0D1F3D1-D14E-407B-9C8C-F414758DE158}"/>
+    <workbookView xWindow="3156" yWindow="600" windowWidth="18996" windowHeight="10392" xr2:uid="{C0D1F3D1-D14E-407B-9C8C-F414758DE158}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="73">
   <si>
     <t>User Authentication Endpoints</t>
   </si>
@@ -195,13 +195,73 @@
   </si>
   <si>
     <t>Financial Goals</t>
+  </si>
+  <si>
+    <t>List all goals of specific user</t>
+  </si>
+  <si>
+    <t>/api/v1/finance/goals</t>
+  </si>
+  <si>
+    <t>Create a new goal</t>
+  </si>
+  <si>
+    <t>Retrieve details of a specific Goal</t>
+  </si>
+  <si>
+    <t>/api/v1/finance/goals/{id}</t>
+  </si>
+  <si>
+    <t>Edit goal</t>
+  </si>
+  <si>
+    <t>Delete a goal</t>
+  </si>
+  <si>
+    <t>Groups`</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>List all groups the authenticated user is a member of.</t>
+  </si>
+  <si>
+    <t>Create a new group (user creating is automatically set as admin).</t>
+  </si>
+  <si>
+    <t>Retrieve details of a specific group, including members and expenses.</t>
+  </si>
+  <si>
+    <t>Update details of a specific group (e.g., name, description).</t>
+  </si>
+  <si>
+    <t>Delete a specific group.</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>Add a user to the group by username (validates if user is already a member).</t>
+  </si>
+  <si>
+    <t>/api/v1/finance/groups/</t>
+  </si>
+  <si>
+    <t>/api/v1/finance/groups/{id}/</t>
+  </si>
+  <si>
+    <t>/api/v1/finance/groups/{id}/add-member/</t>
+  </si>
+  <si>
+    <t>Checked</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +273,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -238,9 +311,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,20 +635,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6071F3C0-484D-4B04-BF47-984C4AE473DE}">
-  <dimension ref="A2:C40"/>
+  <dimension ref="A2:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.109375" customWidth="1"/>
+    <col min="1" max="1" width="37.88671875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="57.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,7 +659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -589,8 +669,11 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -600,8 +683,11 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -611,8 +697,11 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -622,8 +711,11 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -633,8 +725,11 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -645,7 +740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -655,8 +750,11 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -666,8 +764,11 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -677,8 +778,11 @@
       <c r="C12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -688,8 +792,11 @@
       <c r="C13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -699,8 +806,11 @@
       <c r="C14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -711,7 +821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -721,8 +831,11 @@
       <c r="C17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -732,8 +845,11 @@
       <c r="C18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -743,8 +859,11 @@
       <c r="C19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -754,8 +873,11 @@
       <c r="C20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -765,8 +887,11 @@
       <c r="C21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -777,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -787,8 +912,11 @@
       <c r="C24" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -798,8 +926,11 @@
       <c r="C25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -809,8 +940,11 @@
       <c r="C26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -820,8 +954,11 @@
       <c r="C27" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -831,8 +968,11 @@
       <c r="C28" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -842,8 +982,11 @@
       <c r="C30" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -853,8 +996,11 @@
       <c r="C31" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -864,8 +1010,11 @@
       <c r="C32" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -875,8 +1024,11 @@
       <c r="C33" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -886,8 +1038,11 @@
       <c r="C34" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -898,7 +1053,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
@@ -909,7 +1064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -919,8 +1074,14 @@
       <c r="C38" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
@@ -929,6 +1090,163 @@
       </c>
       <c r="C40" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="28.8">
+      <c r="A50" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="28.8">
+      <c r="A53" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>